<commit_message>
Test reports and screenshots
Test reports and screenshots
</commit_message>
<xml_diff>
--- a/Human Resource Management/OrangeHRM_Automation_Test/data/loginData.xlsx
+++ b/Human Resource Management/OrangeHRM_Automation_Test/data/loginData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personals\Vijina\StarAgile\Learning_Materials\Capstone_Projects\Human Resource Management\OrangeHRM_Automation_Test\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personals\Vijina\StarAgile\Learning_Materials\Capstone_Projects\Human_Resources_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EE2202-AB13-4319-A858-932641D02171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1DFDA2-DDCB-4EBD-810A-6141D8CEA8E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Username</t>
   </si>
@@ -37,6 +37,21 @@
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>wrong123</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>pass1</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -80,9 +95,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -391,6 +409,38 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>